<commit_message>
clean push without locked files
</commit_message>
<xml_diff>
--- a/TestData/EmployeeData.xlsx
+++ b/TestData/EmployeeData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\IC_Projects\Excersise\OrangeHRMHybridAutomationFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD49174-E94C-4D4D-8922-A8EFFC794412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93B9EAC-8B91-482A-9480-8EE9549D25E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12525" yWindow="2625" windowWidth="9285" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>John</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Tob</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>EmployeeID</t>
   </si>
 </sst>
 </file>
@@ -369,53 +381,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>123</v>
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>234</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>567</v>
       </c>
     </row>

</xml_diff>